<commit_message>
ata sprint semana c
</commit_message>
<xml_diff>
--- a/Documentação/plano de ação/PlanoDeAção_BeCold - BackUp.xlsx
+++ b/Documentação/plano de ação/PlanoDeAção_BeCold - BackUp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54665B06-14C7-4720-BC02-C5AB43072F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEAD8CD-E219-46CF-8D66-CC6A8CCB57F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do plano de Ação" sheetId="1" r:id="rId1"/>
@@ -32,24 +32,11 @@
     <definedName name="txtPersonalizado4">'Dados do plano de Ação'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="52">
   <si>
     <t>Dados do plano de marketing</t>
   </si>
@@ -189,9 +176,6 @@
     <t>Semana 2-D</t>
   </si>
   <si>
-    <t>Ester, Kaiqui e Paulo</t>
-  </si>
-  <si>
     <t>Thalita e Yuri</t>
   </si>
   <si>
@@ -199,6 +183,15 @@
   </si>
   <si>
     <t>Previsão de término</t>
+  </si>
+  <si>
+    <t>Paulo, Kaiqui</t>
+  </si>
+  <si>
+    <t>Ester, Kaiqui</t>
+  </si>
+  <si>
+    <t>TODOS</t>
   </si>
 </sst>
 </file>
@@ -981,7 +974,7 @@
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1066,9 +1059,6 @@
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="20% - Ênfase1" xfId="7" builtinId="30" customBuiltin="1"/>
@@ -1125,6 +1115,54 @@
     <cellStyle name="Vírgula" xfId="20" builtinId="3" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="52">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1225,42 +1263,6 @@
       <font>
         <b/>
         <i val="0"/>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -1309,18 +1311,6 @@
       <font>
         <b/>
         <i val="0"/>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
         <color theme="6" tint="-0.499984740745262"/>
       </font>
       <fill>
@@ -1338,66 +1328,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1494,6 +1424,66 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6414,6 +6404,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Dados" displayName="Dados" ref="B6:H21" headerRowDxfId="45">
   <autoFilter ref="B6:H21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:H21">
+    <sortCondition ref="D6:D21"/>
+  </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarefa" totalsRowLabel="Total" dataDxfId="44"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Status" totalsRowFunction="count" dataDxfId="43"/>
@@ -6778,10 +6771,10 @@
     <tabColor theme="4" tint="0.39997558519241921"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N21"/>
+  <dimension ref="B1:H21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6871,10 +6864,10 @@
         <v>10</v>
       </c>
       <c r="G6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -6954,19 +6947,19 @@
     </row>
     <row r="10" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="G10" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
@@ -6979,7 +6972,7 @@
     </row>
     <row r="11" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>9</v>
@@ -6991,7 +6984,7 @@
         <v>15</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="G11" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
@@ -7004,227 +6997,244 @@
     </row>
     <row r="12" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="21"/>
+        <v>38</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>50</v>
+      </c>
       <c r="G12" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
-        <v>45178</v>
+        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
+        <v>45171</v>
       </c>
       <c r="H12" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
-        <v>45182</v>
+        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
+        <v>45175</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="21"/>
+        <v>38</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="G13" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
-        <v>45178</v>
+        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
+        <v>45171</v>
       </c>
       <c r="H13" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
-        <v>45182</v>
+        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
+        <v>45175</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="12" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="21"/>
+        <v>38</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="G14" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
-        <v>45178</v>
+        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
+        <v>45171</v>
       </c>
       <c r="H14" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
-        <v>45182</v>
+        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
+        <v>45175</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="21"/>
+        <v>38</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="G15" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
-        <v>45178</v>
+        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
+        <v>45171</v>
       </c>
       <c r="H15" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,13)</f>
-        <v>45182</v>
+        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
+        <v>45175</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="G16" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
-        <v>45171</v>
+        <f ca="1">DATE(YEAR(TODAY()),9,9)</f>
+        <v>45178</v>
       </c>
       <c r="H16" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
-        <v>45175</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,13)</f>
+        <v>45212</v>
       </c>
     </row>
-    <row r="17" spans="2:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="21"/>
+        <v>44</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="G17" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),10,9)</f>
+        <v>45208</v>
+      </c>
+      <c r="H17" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),10,13)</f>
+        <v>45212</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),10,9)</f>
+        <v>45208</v>
+      </c>
+      <c r="H18" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),10,13)</f>
+        <v>45212</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,16)</f>
         <v>45185</v>
       </c>
-      <c r="H17" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,20)</f>
-        <v>45189</v>
+      <c r="H19" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),10,13)</f>
+        <v>45212</v>
       </c>
     </row>
-    <row r="18" spans="2:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="12" t="s">
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),10,9)</f>
+        <v>45208</v>
+      </c>
+      <c r="H20" s="14">
+        <f ca="1">DATE(YEAR(TODAY()),10,20)</f>
+        <v>45219</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D21" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="14">
+      <c r="E21" s="13"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="14">
         <f ca="1">DATE(YEAR(TODAY()),9,16)</f>
         <v>45185</v>
       </c>
-      <c r="H18" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,20)</f>
-        <v>45189</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
-        <v>45171</v>
-      </c>
-      <c r="H19" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
-        <v>45175</v>
-      </c>
-      <c r="N19" s="28"/>
-    </row>
-    <row r="20" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
-        <v>45171</v>
-      </c>
-      <c r="H20" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
-        <v>45175</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,2)</f>
-        <v>45171</v>
-      </c>
       <c r="H21" s="14">
-        <f ca="1">DATE(YEAR(TODAY()),9,6)</f>
-        <v>45175</v>
+        <f ca="1">DATE(YEAR(TODAY()),10,20)</f>
+        <v>45219</v>
       </c>
     </row>
   </sheetData>
@@ -7238,43 +7248,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:C21 E20:H21">
-    <cfRule type="expression" dxfId="30" priority="14">
+    <cfRule type="expression" dxfId="30" priority="9">
+      <formula>($C20="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="10">
+      <formula>($C20="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="11">
+      <formula>($C20="Atrasado")*(clAtrasado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="12">
+      <formula>($C20="Concluído")*(clConcluído="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="13">
+      <formula>(clPersonalizado1="ATIVADO")*($C20=txtPersonalizado1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="14">
       <formula>(clPersonalizado2="ATIVADO")*($C20=txtPersonalizado2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="15">
+    <cfRule type="expression" dxfId="24" priority="15">
       <formula>(clPersonalizado3="ATIVADO")*($C20=txtPersonalizado3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="16">
+    <cfRule type="expression" dxfId="23" priority="16">
       <formula>(clPersonalizado4="ATIVADO")*($C20=txtPersonalizado4)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="9">
-      <formula>($C20="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="10">
-      <formula>($C20="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="11">
-      <formula>($C20="Atrasado")*(clAtrasado="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="12">
-      <formula>($C20="Concluído")*(clConcluído="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="13">
-      <formula>(clPersonalizado1="ATIVADO")*($C20=txtPersonalizado1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D21">
-    <cfRule type="expression" dxfId="22" priority="28">
-      <formula>($C7="Concluído")*(clConcluído="ATIVADO")</formula>
+    <cfRule type="expression" dxfId="22" priority="25">
+      <formula>($C7="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="27">
+    <cfRule type="expression" dxfId="21" priority="26">
+      <formula>($C7="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="27">
       <formula>($C7="Atrasado")*(clAtrasado="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="26">
-      <formula>($C7="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="25">
-      <formula>($C7="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
+    <cfRule type="expression" dxfId="19" priority="28">
+      <formula>($C7="Concluído")*(clConcluído="ATIVADO")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="18" priority="29">
       <formula>(clPersonalizado1="ATIVADO")*($C7=txtPersonalizado1)</formula>
@@ -7290,52 +7300,52 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:H10 B7:C21 E11 G11:H11 E12:H21">
-    <cfRule type="expression" dxfId="14" priority="57">
-      <formula>(clPersonalizado4="ATIVADO")*($C7=txtPersonalizado4)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="45">
+    <cfRule type="expression" dxfId="14" priority="45">
       <formula>($C7="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="46">
+    <cfRule type="expression" dxfId="13" priority="46">
       <formula>($C7="Atrasado")*(clAtrasado="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="52">
+    <cfRule type="expression" dxfId="12" priority="52">
       <formula>($C7="Concluído")*(clConcluído="ATIVADO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="54">
+    <cfRule type="expression" dxfId="11" priority="54">
       <formula>(clPersonalizado1="ATIVADO")*($C7=txtPersonalizado1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="55">
+    <cfRule type="expression" dxfId="10" priority="55">
       <formula>(clPersonalizado2="ATIVADO")*($C7=txtPersonalizado2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="56">
+    <cfRule type="expression" dxfId="9" priority="56">
       <formula>(clPersonalizado3="ATIVADO")*($C7=txtPersonalizado3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="57">
+      <formula>(clPersonalizado4="ATIVADO")*($C7=txtPersonalizado4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>($C11="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>($C11="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>($C11="Atrasado")*(clAtrasado="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>($C11="Concluído")*(clConcluído="ATIVADO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>(clPersonalizado1="ATIVADO")*($C11=txtPersonalizado1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>(clPersonalizado2="ATIVADO")*($C11=txtPersonalizado2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>(clPersonalizado3="ATIVADO")*($C11=txtPersonalizado3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>(clPersonalizado4="ATIVADO")*($C11=txtPersonalizado4)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>($C11="Não Iniciado")*(clNãoIniciado="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>($C11="Em Andamento")*(clEmAndamento="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>($C11="Atrasado")*(clAtrasado="ATIVADO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>($C11="Concluído")*(clConcluído="ATIVADO")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="1742" yWindow="648" count="17">
@@ -7510,6 +7520,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf6cf056b5324d160236e2ac13572175">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="308e4927137fd5e63b6be1bd7725299e" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7729,7 +7748,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -7738,16 +7757,17 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB26FF4A-9A24-42D8-B946-9CA436224F6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ACF481C-B850-47D3-8383-E0C13159DD26}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7767,20 +7787,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99945BEB-7D41-4FB6-9D32-A35A84B455C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB26FF4A-9A24-42D8-B946-9CA436224F6C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>